<commit_message>
Including results from some generic routers
</commit_message>
<xml_diff>
--- a/results/device_listing.xlsx
+++ b/results/device_listing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>HOSTNAME</t>
   </si>
@@ -28,25 +28,40 @@
     <t>TYPE</t>
   </si>
   <si>
-    <t>c9006-jbce-a-clage-1000-tr03-1</t>
-  </si>
-  <si>
-    <t>FOUO_JIE_Router_L3_Switch_V1R1_Manual-xccdf.xml.stig</t>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>U_Network_Perimeter_Router_Cisco_STIG_V8R26_Manual-xccdf.xml.stig</t>
   </si>
   <si>
     <t>CISCO</t>
   </si>
   <si>
-    <t>IOS_XR</t>
-  </si>
-  <si>
-    <t>c9006-jbce-a-patge-2324-127-0104-1</t>
-  </si>
-  <si>
-    <t>c9006-jbce-b-clage-1012-tcf-1</t>
-  </si>
-  <si>
-    <t>c9006-jbce-b-patge-2383-1-0004-1</t>
+    <t>PERIMETER</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>U_Network_Infrastructure_Router_Cisco_STIG_V8R23_Manual-xccdf.xml.stig</t>
+  </si>
+  <si>
+    <t>ROUTER</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>sw1</t>
+  </si>
+  <si>
+    <t>U_Network_L2_Switch_Cisco_STIG_V8R21_Manual-xccdf.xml.stig</t>
+  </si>
+  <si>
+    <t>L2_SWITCH</t>
+  </si>
+  <si>
+    <t>sw2</t>
   </si>
 </sst>
 </file>
@@ -382,7 +397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,41 +443,55 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>